<commit_message>
hieu chinh danh muc chuc nang phan ham thu tuc
</commit_message>
<xml_diff>
--- a/danh muc chuc nang ct ql cap dien.xlsx
+++ b/danh muc chuc nang ct ql cap dien.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="104">
   <si>
     <t>Mã Hiệu</t>
   </si>
@@ -229,6 +229,108 @@
   </si>
   <si>
     <t>Quản lý sơ đồ đường đi nhà khách hàng form mobile</t>
+  </si>
+  <si>
+    <t>Lập trình cho Hàm/ Thủ tục</t>
+  </si>
+  <si>
+    <t>hàm</t>
+  </si>
+  <si>
+    <t>sp_GetThongTinKhachHang</t>
+  </si>
+  <si>
+    <t>sp_GetBCKhaoSat</t>
+  </si>
+  <si>
+    <t>sp_GetThongTinBangChietTinh</t>
+  </si>
+  <si>
+    <t>sp_GetChiTietChiPhiBangChietTinh</t>
+  </si>
+  <si>
+    <t>sp_GetDSVatTu</t>
+  </si>
+  <si>
+    <t>sp_GetDSNhanCong</t>
+  </si>
+  <si>
+    <t>sp_GetDSLienKet</t>
+  </si>
+  <si>
+    <t>sp_GetDSQuyetDinh</t>
+  </si>
+  <si>
+    <t>sp_GetDSHeSo</t>
+  </si>
+  <si>
+    <t>sp_GetDSNhomLoaiCP</t>
+  </si>
+  <si>
+    <t>sp_GetDSMauChietTinh</t>
+  </si>
+  <si>
+    <t>sp_BCDSChietTinh</t>
+  </si>
+  <si>
+    <t>sp_BCBangChietTinh</t>
+  </si>
+  <si>
+    <t>sp_BCKhaoSat</t>
+  </si>
+  <si>
+    <t>sp_BCTongHopVatTu</t>
+  </si>
+  <si>
+    <t>sp_BCQuyetToanVT</t>
+  </si>
+  <si>
+    <t>sp_GetDSNguoiDung</t>
+  </si>
+  <si>
+    <t>sp_GetDSDonVi</t>
+  </si>
+  <si>
+    <t>sp_SetKhachHang</t>
+  </si>
+  <si>
+    <t>sp_SetBangChietTinh</t>
+  </si>
+  <si>
+    <t>sp_SetChiTietCPBangChietTinh</t>
+  </si>
+  <si>
+    <t>sp_SetBCKhaoSat</t>
+  </si>
+  <si>
+    <t>sp_SetVatTu</t>
+  </si>
+  <si>
+    <t>sp_SetNhanCong</t>
+  </si>
+  <si>
+    <t>sp_SetLienKet</t>
+  </si>
+  <si>
+    <t>sp_SetQuyetDinh</t>
+  </si>
+  <si>
+    <t>sp_SetHeSo</t>
+  </si>
+  <si>
+    <t>sp_SetNhomLoaiCP</t>
+  </si>
+  <si>
+    <t>sp_SetMauChietTinh</t>
+  </si>
+  <si>
+    <t>sp_SetNguoiDung</t>
+  </si>
+  <si>
+    <t>sp_SetDonVI</t>
+  </si>
+  <si>
+    <t>sp_GetDSKhachHang</t>
   </si>
 </sst>
 </file>
@@ -756,7 +858,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -764,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C289"/>
+  <dimension ref="A1:C304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:C101"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122:XFD122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,253 +1692,383 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="19"/>
-      <c r="B96" s="20"/>
+      <c r="B96" s="31" t="s">
+        <v>70</v>
+      </c>
       <c r="C96" s="8"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="19"/>
-      <c r="B97" s="20"/>
-      <c r="C97" s="8"/>
+      <c r="B97" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="19"/>
-      <c r="B98" s="20"/>
-      <c r="C98" s="8"/>
+      <c r="B98" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="19"/>
-      <c r="B99" s="20"/>
-      <c r="C99" s="8"/>
+      <c r="B99" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="19"/>
-      <c r="B100" s="20"/>
-      <c r="C100" s="8"/>
+      <c r="B100" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="19"/>
-      <c r="B101" s="20"/>
-      <c r="C101" s="8"/>
+      <c r="B101" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="19"/>
-      <c r="B102" s="20"/>
-      <c r="C102" s="8"/>
+      <c r="B102" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="19"/>
-      <c r="B103" s="20"/>
-      <c r="C103" s="8"/>
+      <c r="B103" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="19"/>
-      <c r="B104" s="20"/>
-      <c r="C104" s="8"/>
+      <c r="B104" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="19"/>
-      <c r="B105" s="20"/>
-      <c r="C105" s="8"/>
+      <c r="B105" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="19"/>
-      <c r="B106" s="20"/>
-      <c r="C106" s="8"/>
+      <c r="B106" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="19"/>
-      <c r="B107" s="20"/>
-      <c r="C107" s="8"/>
+      <c r="B107" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="19"/>
-      <c r="B108" s="20"/>
-      <c r="C108" s="8"/>
+      <c r="B108" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="19"/>
-      <c r="B109" s="20"/>
-      <c r="C109" s="8"/>
+      <c r="B109" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="19"/>
-      <c r="B110" s="20"/>
-      <c r="C110" s="8"/>
+      <c r="B110" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="19"/>
-      <c r="B111" s="20"/>
-      <c r="C111" s="8"/>
+      <c r="B111" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="19"/>
-      <c r="B112" s="20"/>
-      <c r="C112" s="8"/>
+      <c r="B112" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="19"/>
-      <c r="B113" s="20"/>
-      <c r="C113" s="8"/>
+      <c r="B113" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="19"/>
-      <c r="B114" s="20"/>
-      <c r="C114" s="8"/>
+      <c r="B114" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="19"/>
-      <c r="B115" s="20"/>
-      <c r="C115" s="8"/>
+      <c r="B115" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="19"/>
-      <c r="B116" s="20"/>
-      <c r="C116" s="8"/>
+      <c r="B116" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="19"/>
-      <c r="B117" s="20"/>
-      <c r="C117" s="8"/>
+      <c r="B117" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="19"/>
-      <c r="B118" s="20"/>
-      <c r="C118" s="8"/>
+      <c r="B118" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="19"/>
-      <c r="B119" s="20"/>
-      <c r="C119" s="8"/>
+      <c r="B119" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="19"/>
-      <c r="B120" s="20"/>
-      <c r="C120" s="8"/>
+      <c r="B120" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="19"/>
-      <c r="B121" s="20"/>
-      <c r="C121" s="8"/>
+      <c r="B121" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="19"/>
-      <c r="B122" s="20"/>
-      <c r="C122" s="8"/>
+      <c r="B122" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="22"/>
-      <c r="B123" s="23"/>
-      <c r="C123" s="5"/>
+      <c r="A123" s="19"/>
+      <c r="B123" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="19"/>
-      <c r="B124" s="24"/>
-      <c r="C124" s="8"/>
+      <c r="B124" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="19"/>
-      <c r="B125" s="24"/>
-      <c r="C125" s="8"/>
+      <c r="B125" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="19"/>
-      <c r="B126" s="24"/>
-      <c r="C126" s="8"/>
+      <c r="B126" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="19"/>
-      <c r="B127" s="24"/>
-      <c r="C127" s="8"/>
+      <c r="B127" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="19"/>
-      <c r="B128" s="24"/>
-      <c r="C128" s="8"/>
+      <c r="B128" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="19"/>
-      <c r="B129" s="24"/>
+      <c r="B129" s="20"/>
       <c r="C129" s="8"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="19"/>
-      <c r="B130" s="24"/>
+      <c r="B130" s="20"/>
       <c r="C130" s="8"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="25"/>
-      <c r="B131" s="26"/>
-      <c r="C131" s="17"/>
+      <c r="A131" s="19"/>
+      <c r="B131" s="20"/>
+      <c r="C131" s="8"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="25"/>
-      <c r="B132" s="26"/>
-      <c r="C132" s="17"/>
+      <c r="A132" s="19"/>
+      <c r="B132" s="20"/>
+      <c r="C132" s="8"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="19"/>
-      <c r="B133" s="24"/>
+      <c r="B133" s="20"/>
       <c r="C133" s="8"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="19"/>
-      <c r="B134" s="10"/>
+      <c r="B134" s="20"/>
       <c r="C134" s="8"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="19"/>
-      <c r="B135" s="10"/>
+      <c r="B135" s="20"/>
       <c r="C135" s="8"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="19"/>
-      <c r="B136" s="10"/>
+      <c r="B136" s="20"/>
       <c r="C136" s="8"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="19"/>
-      <c r="B137" s="10"/>
+      <c r="B137" s="20"/>
       <c r="C137" s="8"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="19"/>
-      <c r="B138" s="10"/>
+      <c r="A138" s="22"/>
+      <c r="B138" s="20"/>
       <c r="C138" s="8"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="25"/>
-      <c r="B139" s="16"/>
-      <c r="C139" s="17"/>
+      <c r="A139" s="19"/>
+      <c r="B139" s="20"/>
+      <c r="C139" s="8"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="25"/>
-      <c r="B140" s="16"/>
-      <c r="C140" s="17"/>
+      <c r="A140" s="19"/>
+      <c r="B140" s="20"/>
+      <c r="C140" s="8"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="25"/>
-      <c r="B141" s="16"/>
-      <c r="C141" s="17"/>
+      <c r="A141" s="19"/>
+      <c r="B141" s="20"/>
+      <c r="C141" s="8"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="19"/>
-      <c r="B142" s="24"/>
+      <c r="B142" s="20"/>
       <c r="C142" s="8"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="19"/>
-      <c r="B143" s="24"/>
+      <c r="B143" s="20"/>
       <c r="C143" s="8"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="25"/>
-      <c r="B144" s="26"/>
-      <c r="C144" s="17"/>
+      <c r="A144" s="19"/>
+      <c r="B144" s="20"/>
+      <c r="C144" s="8"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="25"/>
-      <c r="B145" s="26"/>
-      <c r="C145" s="17"/>
+      <c r="A145" s="19"/>
+      <c r="B145" s="20"/>
+      <c r="C145" s="8"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="25"/>
@@ -1844,9 +2076,9 @@
       <c r="C146" s="17"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="19"/>
-      <c r="B147" s="24"/>
-      <c r="C147" s="8"/>
+      <c r="A147" s="25"/>
+      <c r="B147" s="26"/>
+      <c r="C147" s="17"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="19"/>
@@ -1854,13 +2086,13 @@
       <c r="C148" s="8"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="27"/>
-      <c r="B149" s="4"/>
-      <c r="C149" s="5"/>
+      <c r="A149" s="19"/>
+      <c r="B149" s="10"/>
+      <c r="C149" s="8"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="19"/>
-      <c r="B150" s="7"/>
+      <c r="B150" s="10"/>
       <c r="C150" s="8"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -1874,14 +2106,14 @@
       <c r="C152" s="8"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="25"/>
-      <c r="B153" s="16"/>
+      <c r="A153" s="19"/>
+      <c r="B153" s="10"/>
       <c r="C153" s="8"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="19"/>
-      <c r="B154" s="10"/>
-      <c r="C154" s="8"/>
+      <c r="A154" s="25"/>
+      <c r="B154" s="16"/>
+      <c r="C154" s="17"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="25"/>
@@ -1889,53 +2121,53 @@
       <c r="C155" s="17"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="19"/>
-      <c r="B156" s="10"/>
-      <c r="C156" s="8"/>
+      <c r="A156" s="25"/>
+      <c r="B156" s="16"/>
+      <c r="C156" s="17"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="19"/>
-      <c r="B157" s="10"/>
+      <c r="B157" s="24"/>
       <c r="C157" s="8"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="19"/>
-      <c r="B158" s="10"/>
+      <c r="B158" s="24"/>
       <c r="C158" s="8"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="25"/>
-      <c r="B159" s="16"/>
-      <c r="C159" s="8"/>
+      <c r="B159" s="26"/>
+      <c r="C159" s="17"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="25"/>
-      <c r="B160" s="16"/>
+      <c r="B160" s="26"/>
       <c r="C160" s="17"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="19"/>
-      <c r="B161" s="7"/>
-      <c r="C161" s="8"/>
+      <c r="A161" s="25"/>
+      <c r="B161" s="26"/>
+      <c r="C161" s="17"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="19"/>
-      <c r="B162" s="12"/>
+      <c r="B162" s="24"/>
       <c r="C162" s="8"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="19"/>
-      <c r="B163" s="10"/>
+      <c r="B163" s="24"/>
       <c r="C163" s="8"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="25"/>
-      <c r="B164" s="16"/>
-      <c r="C164" s="17"/>
+      <c r="A164" s="27"/>
+      <c r="B164" s="4"/>
+      <c r="C164" s="5"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="19"/>
-      <c r="B165" s="10"/>
+      <c r="B165" s="7"/>
       <c r="C165" s="8"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -1945,12 +2177,12 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="19"/>
-      <c r="B167" s="7"/>
+      <c r="B167" s="10"/>
       <c r="C167" s="8"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="19"/>
-      <c r="B168" s="10"/>
+      <c r="A168" s="25"/>
+      <c r="B168" s="16"/>
       <c r="C168" s="8"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -1964,119 +2196,119 @@
       <c r="C170" s="17"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="25"/>
-      <c r="B171" s="16"/>
-      <c r="C171" s="17"/>
+      <c r="A171" s="19"/>
+      <c r="B171" s="10"/>
+      <c r="C171" s="8"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="25"/>
-      <c r="B172" s="16"/>
-      <c r="C172" s="17"/>
+      <c r="A172" s="19"/>
+      <c r="B172" s="10"/>
+      <c r="C172" s="8"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="25"/>
-      <c r="B173" s="16"/>
-      <c r="C173" s="17"/>
+      <c r="A173" s="19"/>
+      <c r="B173" s="10"/>
+      <c r="C173" s="8"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="19"/>
-      <c r="B174" s="10"/>
+      <c r="A174" s="25"/>
+      <c r="B174" s="16"/>
       <c r="C174" s="8"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="19"/>
-      <c r="B175" s="7"/>
-      <c r="C175" s="8"/>
+      <c r="A175" s="25"/>
+      <c r="B175" s="16"/>
+      <c r="C175" s="17"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="19"/>
-      <c r="B176" s="10"/>
+      <c r="B176" s="7"/>
       <c r="C176" s="8"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="19"/>
-      <c r="B177" s="10"/>
+      <c r="B177" s="12"/>
       <c r="C177" s="8"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="23"/>
-      <c r="B178" s="23"/>
-      <c r="C178" s="21"/>
+      <c r="A178" s="19"/>
+      <c r="B178" s="10"/>
+      <c r="C178" s="8"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="19"/>
-      <c r="B179" s="20"/>
-      <c r="C179" s="8"/>
+      <c r="A179" s="25"/>
+      <c r="B179" s="16"/>
+      <c r="C179" s="17"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="19"/>
-      <c r="B180" s="20"/>
+      <c r="B180" s="10"/>
       <c r="C180" s="8"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="19"/>
-      <c r="B181" s="20"/>
+      <c r="B181" s="10"/>
       <c r="C181" s="8"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="19"/>
-      <c r="B182" s="20"/>
+      <c r="B182" s="7"/>
       <c r="C182" s="8"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="19"/>
-      <c r="B183" s="20"/>
+      <c r="B183" s="10"/>
       <c r="C183" s="8"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="19"/>
-      <c r="B184" s="20"/>
+      <c r="B184" s="10"/>
       <c r="C184" s="8"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="19"/>
-      <c r="B185" s="20"/>
-      <c r="C185" s="8"/>
+      <c r="A185" s="25"/>
+      <c r="B185" s="16"/>
+      <c r="C185" s="17"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="19"/>
-      <c r="B186" s="20"/>
-      <c r="C186" s="8"/>
+      <c r="A186" s="25"/>
+      <c r="B186" s="16"/>
+      <c r="C186" s="17"/>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" s="19"/>
-      <c r="B187" s="20"/>
-      <c r="C187" s="8"/>
+      <c r="A187" s="25"/>
+      <c r="B187" s="16"/>
+      <c r="C187" s="17"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="19"/>
-      <c r="B188" s="20"/>
-      <c r="C188" s="8"/>
+      <c r="A188" s="25"/>
+      <c r="B188" s="16"/>
+      <c r="C188" s="17"/>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="19"/>
-      <c r="B189" s="20"/>
+      <c r="B189" s="10"/>
       <c r="C189" s="8"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="19"/>
-      <c r="B190" s="20"/>
+      <c r="B190" s="7"/>
       <c r="C190" s="8"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="19"/>
-      <c r="B191" s="20"/>
+      <c r="B191" s="10"/>
       <c r="C191" s="8"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="19"/>
-      <c r="B192" s="20"/>
+      <c r="B192" s="10"/>
       <c r="C192" s="8"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="19"/>
-      <c r="B193" s="20"/>
-      <c r="C193" s="8"/>
+      <c r="A193" s="23"/>
+      <c r="B193" s="23"/>
+      <c r="C193" s="21"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="19"/>
@@ -2174,99 +2406,99 @@
       <c r="C212" s="8"/>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" s="27"/>
-      <c r="B213" s="23"/>
-      <c r="C213" s="5"/>
+      <c r="A213" s="19"/>
+      <c r="B213" s="20"/>
+      <c r="C213" s="8"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="19"/>
-      <c r="B214" s="24"/>
+      <c r="B214" s="20"/>
       <c r="C214" s="8"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="19"/>
-      <c r="B215" s="24"/>
+      <c r="B215" s="20"/>
       <c r="C215" s="8"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="19"/>
-      <c r="B216" s="24"/>
+      <c r="B216" s="20"/>
       <c r="C216" s="8"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="19"/>
-      <c r="B217" s="24"/>
+      <c r="B217" s="20"/>
       <c r="C217" s="8"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="19"/>
-      <c r="B218" s="24"/>
+      <c r="B218" s="20"/>
       <c r="C218" s="8"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="19"/>
-      <c r="B219" s="24"/>
+      <c r="B219" s="20"/>
       <c r="C219" s="8"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="19"/>
-      <c r="B220" s="24"/>
+      <c r="B220" s="20"/>
       <c r="C220" s="8"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" s="25"/>
-      <c r="B221" s="26"/>
-      <c r="C221" s="17"/>
+      <c r="A221" s="19"/>
+      <c r="B221" s="20"/>
+      <c r="C221" s="8"/>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" s="25"/>
-      <c r="B222" s="26"/>
-      <c r="C222" s="17"/>
+      <c r="A222" s="19"/>
+      <c r="B222" s="20"/>
+      <c r="C222" s="8"/>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="19"/>
-      <c r="B223" s="24"/>
+      <c r="B223" s="20"/>
       <c r="C223" s="8"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="19"/>
-      <c r="B224" s="10"/>
+      <c r="B224" s="20"/>
       <c r="C224" s="8"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="19"/>
-      <c r="B225" s="10"/>
+      <c r="B225" s="20"/>
       <c r="C225" s="8"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="19"/>
-      <c r="B226" s="10"/>
+      <c r="B226" s="20"/>
       <c r="C226" s="8"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="19"/>
-      <c r="B227" s="10"/>
+      <c r="B227" s="20"/>
       <c r="C227" s="8"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="19"/>
-      <c r="B228" s="10"/>
-      <c r="C228" s="8"/>
+      <c r="A228" s="27"/>
+      <c r="B228" s="23"/>
+      <c r="C228" s="5"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" s="25"/>
-      <c r="B229" s="16"/>
-      <c r="C229" s="17"/>
+      <c r="A229" s="19"/>
+      <c r="B229" s="24"/>
+      <c r="C229" s="8"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="19"/>
-      <c r="B230" s="10"/>
+      <c r="B230" s="24"/>
       <c r="C230" s="8"/>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231" s="25"/>
-      <c r="B231" s="16"/>
-      <c r="C231" s="17"/>
+      <c r="A231" s="19"/>
+      <c r="B231" s="24"/>
+      <c r="C231" s="8"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="19"/>
@@ -2279,14 +2511,14 @@
       <c r="C233" s="8"/>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" s="25"/>
-      <c r="B234" s="26"/>
-      <c r="C234" s="17"/>
+      <c r="A234" s="19"/>
+      <c r="B234" s="24"/>
+      <c r="C234" s="8"/>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" s="25"/>
-      <c r="B235" s="26"/>
-      <c r="C235" s="17"/>
+      <c r="A235" s="19"/>
+      <c r="B235" s="24"/>
+      <c r="C235" s="8"/>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="25"/>
@@ -2294,9 +2526,9 @@
       <c r="C236" s="17"/>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" s="19"/>
-      <c r="B237" s="24"/>
-      <c r="C237" s="8"/>
+      <c r="A237" s="25"/>
+      <c r="B237" s="26"/>
+      <c r="C237" s="17"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="19"/>
@@ -2304,13 +2536,13 @@
       <c r="C238" s="8"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" s="27"/>
-      <c r="B239" s="4"/>
-      <c r="C239" s="5"/>
+      <c r="A239" s="19"/>
+      <c r="B239" s="10"/>
+      <c r="C239" s="8"/>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="19"/>
-      <c r="B240" s="7"/>
+      <c r="B240" s="10"/>
       <c r="C240" s="8"/>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -2324,49 +2556,49 @@
       <c r="C242" s="8"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="25"/>
-      <c r="B243" s="16"/>
-      <c r="C243" s="17"/>
+      <c r="A243" s="19"/>
+      <c r="B243" s="10"/>
+      <c r="C243" s="8"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="19"/>
-      <c r="B244" s="10"/>
-      <c r="C244" s="8"/>
+      <c r="A244" s="25"/>
+      <c r="B244" s="16"/>
+      <c r="C244" s="17"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" s="25"/>
-      <c r="B245" s="16"/>
-      <c r="C245" s="17"/>
+      <c r="A245" s="19"/>
+      <c r="B245" s="10"/>
+      <c r="C245" s="8"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246" s="19"/>
-      <c r="B246" s="10"/>
-      <c r="C246" s="8"/>
+      <c r="A246" s="25"/>
+      <c r="B246" s="16"/>
+      <c r="C246" s="17"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="19"/>
-      <c r="B247" s="10"/>
+      <c r="B247" s="24"/>
       <c r="C247" s="8"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="19"/>
-      <c r="B248" s="10"/>
+      <c r="B248" s="24"/>
       <c r="C248" s="8"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="25"/>
-      <c r="B249" s="16"/>
+      <c r="B249" s="26"/>
       <c r="C249" s="17"/>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250" s="19"/>
-      <c r="B250" s="10"/>
-      <c r="C250" s="8"/>
+      <c r="A250" s="25"/>
+      <c r="B250" s="26"/>
+      <c r="C250" s="17"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" s="19"/>
-      <c r="B251" s="28"/>
-      <c r="C251" s="8"/>
+      <c r="A251" s="25"/>
+      <c r="B251" s="26"/>
+      <c r="C251" s="17"/>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="19"/>
@@ -2374,44 +2606,44 @@
       <c r="C252" s="8"/>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" s="25"/>
-      <c r="B253" s="26"/>
-      <c r="C253" s="17"/>
+      <c r="A253" s="19"/>
+      <c r="B253" s="24"/>
+      <c r="C253" s="8"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254" s="25"/>
-      <c r="B254" s="26"/>
-      <c r="C254" s="17"/>
+      <c r="A254" s="27"/>
+      <c r="B254" s="4"/>
+      <c r="C254" s="5"/>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="19"/>
-      <c r="B255" s="24"/>
+      <c r="B255" s="7"/>
       <c r="C255" s="8"/>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="19"/>
-      <c r="B256" s="14"/>
+      <c r="B256" s="10"/>
       <c r="C256" s="8"/>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="19"/>
-      <c r="B257" s="12"/>
+      <c r="B257" s="10"/>
       <c r="C257" s="8"/>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" s="19"/>
-      <c r="B258" s="10"/>
-      <c r="C258" s="8"/>
+      <c r="A258" s="25"/>
+      <c r="B258" s="16"/>
+      <c r="C258" s="17"/>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" s="25"/>
-      <c r="B259" s="16"/>
-      <c r="C259" s="17"/>
+      <c r="A259" s="19"/>
+      <c r="B259" s="10"/>
+      <c r="C259" s="8"/>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" s="19"/>
-      <c r="B260" s="10"/>
-      <c r="C260" s="8"/>
+      <c r="A260" s="25"/>
+      <c r="B260" s="16"/>
+      <c r="C260" s="17"/>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="19"/>
@@ -2420,7 +2652,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="19"/>
-      <c r="B262" s="13"/>
+      <c r="B262" s="10"/>
       <c r="C262" s="8"/>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -2429,9 +2661,9 @@
       <c r="C263" s="8"/>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" s="19"/>
-      <c r="B264" s="10"/>
-      <c r="C264" s="8"/>
+      <c r="A264" s="25"/>
+      <c r="B264" s="16"/>
+      <c r="C264" s="17"/>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="19"/>
@@ -2440,37 +2672,37 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="19"/>
-      <c r="B266" s="7"/>
+      <c r="B266" s="28"/>
       <c r="C266" s="8"/>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="19"/>
-      <c r="B267" s="10"/>
+      <c r="B267" s="24"/>
       <c r="C267" s="8"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A268" s="19"/>
-      <c r="B268" s="10"/>
-      <c r="C268" s="8"/>
+      <c r="A268" s="25"/>
+      <c r="B268" s="26"/>
+      <c r="C268" s="17"/>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="25"/>
-      <c r="B269" s="16"/>
+      <c r="B269" s="26"/>
       <c r="C269" s="17"/>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="25"/>
-      <c r="B270" s="16"/>
-      <c r="C270" s="17"/>
+      <c r="A270" s="19"/>
+      <c r="B270" s="24"/>
+      <c r="C270" s="8"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A271" s="25"/>
-      <c r="B271" s="16"/>
-      <c r="C271" s="17"/>
+      <c r="A271" s="19"/>
+      <c r="B271" s="14"/>
+      <c r="C271" s="8"/>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="19"/>
-      <c r="B272" s="10"/>
+      <c r="B272" s="12"/>
       <c r="C272" s="8"/>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -2479,14 +2711,14 @@
       <c r="C273" s="8"/>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A274" s="19"/>
-      <c r="B274" s="10"/>
-      <c r="C274" s="8"/>
+      <c r="A274" s="25"/>
+      <c r="B274" s="16"/>
+      <c r="C274" s="17"/>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A275" s="25"/>
-      <c r="B275" s="16"/>
-      <c r="C275" s="17"/>
+      <c r="A275" s="19"/>
+      <c r="B275" s="10"/>
+      <c r="C275" s="8"/>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="19"/>
@@ -2494,73 +2726,148 @@
       <c r="C276" s="8"/>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A277" s="25"/>
-      <c r="B277" s="16"/>
-      <c r="C277" s="17"/>
+      <c r="A277" s="19"/>
+      <c r="B277" s="13"/>
+      <c r="C277" s="8"/>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="19"/>
-      <c r="B278" s="13"/>
+      <c r="B278" s="10"/>
       <c r="C278" s="8"/>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="19"/>
-      <c r="B279" s="24"/>
+      <c r="B279" s="10"/>
       <c r="C279" s="8"/>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="19"/>
-      <c r="B280" s="24"/>
+      <c r="B280" s="10"/>
       <c r="C280" s="8"/>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" s="25"/>
-      <c r="B281" s="26"/>
+      <c r="A281" s="19"/>
+      <c r="B281" s="7"/>
       <c r="C281" s="8"/>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" s="25"/>
-      <c r="B282" s="26"/>
-      <c r="C282" s="17"/>
+      <c r="A282" s="19"/>
+      <c r="B282" s="10"/>
+      <c r="C282" s="8"/>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A283" s="25"/>
-      <c r="B283" s="26"/>
-      <c r="C283" s="17"/>
+      <c r="A283" s="19"/>
+      <c r="B283" s="10"/>
+      <c r="C283" s="8"/>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A284" s="19"/>
-      <c r="B284" s="7"/>
-      <c r="C284" s="8"/>
+      <c r="A284" s="25"/>
+      <c r="B284" s="16"/>
+      <c r="C284" s="17"/>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A285" s="19"/>
-      <c r="B285" s="10"/>
-      <c r="C285" s="8"/>
+      <c r="A285" s="25"/>
+      <c r="B285" s="16"/>
+      <c r="C285" s="17"/>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A286" s="19"/>
-      <c r="B286" s="10"/>
-      <c r="C286" s="8"/>
+      <c r="A286" s="25"/>
+      <c r="B286" s="16"/>
+      <c r="C286" s="17"/>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A287" s="29"/>
-      <c r="B287" s="4"/>
-      <c r="C287" s="5"/>
+      <c r="A287" s="19"/>
+      <c r="B287" s="10"/>
+      <c r="C287" s="8"/>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" s="29"/>
-      <c r="B288" s="4"/>
-      <c r="C288" s="5"/>
+      <c r="A288" s="19"/>
+      <c r="B288" s="10"/>
+      <c r="C288" s="8"/>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A289" s="32"/>
-      <c r="B289" s="33"/>
+      <c r="A289" s="19"/>
+      <c r="B289" s="10"/>
       <c r="C289" s="8"/>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" s="25"/>
+      <c r="B290" s="16"/>
+      <c r="C290" s="17"/>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" s="19"/>
+      <c r="B291" s="10"/>
+      <c r="C291" s="8"/>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="25"/>
+      <c r="B292" s="16"/>
+      <c r="C292" s="17"/>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" s="19"/>
+      <c r="B293" s="13"/>
+      <c r="C293" s="8"/>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="19"/>
+      <c r="B294" s="24"/>
+      <c r="C294" s="8"/>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" s="19"/>
+      <c r="B295" s="24"/>
+      <c r="C295" s="8"/>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" s="25"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="8"/>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" s="25"/>
+      <c r="B297" s="26"/>
+      <c r="C297" s="17"/>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" s="25"/>
+      <c r="B298" s="26"/>
+      <c r="C298" s="17"/>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" s="19"/>
+      <c r="B299" s="7"/>
+      <c r="C299" s="8"/>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="19"/>
+      <c r="B300" s="10"/>
+      <c r="C300" s="8"/>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" s="19"/>
+      <c r="B301" s="10"/>
+      <c r="C301" s="8"/>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" s="29"/>
+      <c r="B302" s="4"/>
+      <c r="C302" s="5"/>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" s="29"/>
+      <c r="B303" s="4"/>
+      <c r="C303" s="5"/>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" s="32"/>
+      <c r="B304" s="33"/>
+      <c r="C304" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A289:B289"/>
+    <mergeCell ref="A304:B304"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
   </mergeCells>

</xml_diff>